<commit_message>
Update 1.0A extruder thermistor table
Update 1.0A extruder thermistor table to fix sensor defect error when
temperature is around and under 20 degres - thanks superdavex
</commit_message>
<xml_diff>
--- a/bed-extruder-tables.xlsx
+++ b/bed-extruder-tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bed" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <definedName name="bed1_" localSheetId="0">Bed!$A$80:$B$95</definedName>
     <definedName name="extruder0" localSheetId="1">'Extruder gen 0'!$A$3:$B$30</definedName>
     <definedName name="extruder0_pcb_man" localSheetId="1">'Extruder gen 0'!$A$35:$B$74</definedName>
-    <definedName name="extruder1" localSheetId="2">'Extruder gen 1'!$A$3:$B$29</definedName>
+    <definedName name="extruder1" localSheetId="2">'Extruder gen 1'!$A$3:$B$30</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -144,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -887,11 +887,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91758976"/>
-        <c:axId val="91760512"/>
+        <c:axId val="91271552"/>
+        <c:axId val="91273088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91758976"/>
+        <c:axId val="91271552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -901,12 +901,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91760512"/>
+        <c:crossAx val="91273088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91760512"/>
+        <c:axId val="91273088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -917,7 +917,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91758976"/>
+        <c:crossAx val="91271552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1632,11 +1632,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91792512"/>
-        <c:axId val="91794048"/>
+        <c:axId val="91509888"/>
+        <c:axId val="91511424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91792512"/>
+        <c:axId val="91509888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="160"/>
@@ -1648,12 +1648,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91794048"/>
+        <c:crossAx val="91511424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91794048"/>
+        <c:axId val="91511424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4500"/>
@@ -1666,14 +1666,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91792512"/>
+        <c:crossAx val="91509888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2224,11 +2223,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="93040640"/>
-        <c:axId val="93042560"/>
+        <c:axId val="91631616"/>
+        <c:axId val="91633536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93040640"/>
+        <c:axId val="91631616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="160"/>
@@ -2240,12 +2239,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93042560"/>
+        <c:crossAx val="91633536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93042560"/>
+        <c:axId val="91633536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2256,14 +2255,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93040640"/>
+        <c:crossAx val="91631616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2313,7 +2311,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2742,11 +2739,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="93060096"/>
-        <c:axId val="93065984"/>
+        <c:axId val="91646976"/>
+        <c:axId val="91652864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93060096"/>
+        <c:axId val="91646976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="160"/>
@@ -2758,12 +2755,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93065984"/>
+        <c:crossAx val="91652864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93065984"/>
+        <c:axId val="91652864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2774,14 +2771,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93060096"/>
+        <c:crossAx val="91646976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2826,7 +2822,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3553,11 +3548,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="90898816"/>
-        <c:axId val="90900352"/>
+        <c:axId val="90986368"/>
+        <c:axId val="90987904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90898816"/>
+        <c:axId val="90986368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -3569,12 +3564,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90900352"/>
+        <c:crossAx val="90987904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90900352"/>
+        <c:axId val="90987904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3585,14 +3580,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90898816"/>
+        <c:crossAx val="90986368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3642,7 +3636,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4149,11 +4142,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="90930176"/>
-        <c:axId val="90936064"/>
+        <c:axId val="91026176"/>
+        <c:axId val="91027712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90930176"/>
+        <c:axId val="91026176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4163,12 +4156,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90936064"/>
+        <c:crossAx val="91027712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90936064"/>
+        <c:axId val="91027712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4179,14 +4172,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90930176"/>
+        <c:crossAx val="91026176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4261,10 +4253,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Extruder gen 1'!$E$3:$E$29</c:f>
+              <c:f>'Extruder gen 1'!$E$3:$E$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>320</c:v>
                 </c:pt>
@@ -4341,9 +4333,12 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>-20</c:v>
                 </c:pt>
               </c:numCache>
@@ -4351,10 +4346,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Extruder gen 1'!$F$3:$F$29</c:f>
+              <c:f>'Extruder gen 1'!$F$3:$F$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>294</c:v>
                 </c:pt>
@@ -4431,10 +4426,13 @@
                   <c:v>4067</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4076</c:v>
+                  <c:v>4079</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4081</c:v>
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4449,11 +4447,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="90952832"/>
-        <c:axId val="90954368"/>
+        <c:axId val="91093632"/>
+        <c:axId val="92356992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90952832"/>
+        <c:axId val="91093632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -4465,12 +4463,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90954368"/>
+        <c:crossAx val="92356992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90954368"/>
+        <c:axId val="92356992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4481,7 +4479,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90952832"/>
+        <c:crossAx val="91093632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4702,7 +4700,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4726,15 +4724,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bed0-david" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bed0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bed1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bed0-david" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5042,7 +5040,7 @@
       <selection activeCell="E124" sqref="E124:I142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
@@ -5050,12 +5048,12 @@
     <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5069,7 +5067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2003</v>
       </c>
@@ -5085,7 +5083,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2058</v>
       </c>
@@ -5101,7 +5099,7 @@
         <v>2058</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2161</v>
       </c>
@@ -5117,7 +5115,7 @@
         <v>2161</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2253</v>
       </c>
@@ -5133,7 +5131,7 @@
         <v>2253</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2337</v>
       </c>
@@ -5149,7 +5147,7 @@
         <v>2337</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2450</v>
       </c>
@@ -5165,7 +5163,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2549</v>
       </c>
@@ -5181,7 +5179,7 @@
         <v>2549</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2637</v>
       </c>
@@ -5197,7 +5195,7 @@
         <v>2637</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2715</v>
       </c>
@@ -5213,7 +5211,7 @@
         <v>2715</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2786</v>
       </c>
@@ -5229,7 +5227,7 @@
         <v>2786</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2907</v>
       </c>
@@ -5245,7 +5243,7 @@
         <v>2907</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3008</v>
       </c>
@@ -5261,7 +5259,7 @@
         <v>3008</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3093</v>
       </c>
@@ -5277,7 +5275,7 @@
         <v>3093</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3165</v>
       </c>
@@ -5293,7 +5291,7 @@
         <v>3165</v>
       </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3247</v>
       </c>
@@ -5309,7 +5307,7 @@
         <v>3247</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3316</v>
       </c>
@@ -5331,7 +5329,7 @@
         <v>3708</v>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3374</v>
       </c>
@@ -5353,7 +5351,7 @@
         <v>3816</v>
       </c>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3447</v>
       </c>
@@ -5375,7 +5373,7 @@
         <v>3920</v>
       </c>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3506</v>
       </c>
@@ -5397,7 +5395,7 @@
         <v>4025</v>
       </c>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3548</v>
       </c>
@@ -5419,7 +5417,7 @@
         <v>4129</v>
       </c>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3610</v>
       </c>
@@ -5435,7 +5433,7 @@
         <v>3610</v>
       </c>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3664</v>
       </c>
@@ -5451,7 +5449,7 @@
         <v>3664</v>
       </c>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3708</v>
       </c>
@@ -5467,7 +5465,7 @@
         <v>3708</v>
       </c>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3764</v>
       </c>
@@ -5483,7 +5481,7 @@
         <v>3764</v>
       </c>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3816</v>
       </c>
@@ -5499,7 +5497,7 @@
         <v>3816</v>
       </c>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3868</v>
       </c>
@@ -5515,7 +5513,7 @@
         <v>3868</v>
       </c>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3920</v>
       </c>
@@ -5531,7 +5529,7 @@
         <v>3920</v>
       </c>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4025</v>
       </c>
@@ -5547,7 +5545,7 @@
         <v>4025</v>
       </c>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4129</v>
       </c>
@@ -5563,7 +5561,7 @@
         <v>4129</v>
       </c>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4233</v>
       </c>
@@ -5579,12 +5577,12 @@
         <v>4233</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -5598,7 +5596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -5615,7 +5613,7 @@
       </c>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>180</v>
       </c>
@@ -5631,7 +5629,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>356</v>
       </c>
@@ -5647,7 +5645,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>532</v>
       </c>
@@ -5663,7 +5661,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>708</v>
       </c>
@@ -5679,7 +5677,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>884</v>
       </c>
@@ -5695,7 +5693,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1295</v>
       </c>
@@ -5711,7 +5709,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1306</v>
       </c>
@@ -5727,7 +5725,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1323</v>
       </c>
@@ -5743,7 +5741,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1557</v>
       </c>
@@ -5759,7 +5757,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1755</v>
       </c>
@@ -5776,7 +5774,7 @@
         <v>1755</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2005</v>
       </c>
@@ -5793,7 +5791,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2090</v>
       </c>
@@ -5810,7 +5808,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2151</v>
       </c>
@@ -5827,7 +5825,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2231</v>
       </c>
@@ -5844,7 +5842,7 @@
         <v>2231</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2330</v>
       </c>
@@ -5861,7 +5859,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2398</v>
       </c>
@@ -5878,7 +5876,7 @@
         <v>2398</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2482</v>
       </c>
@@ -5895,7 +5893,7 @@
         <v>2482</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2561</v>
       </c>
@@ -5912,7 +5910,7 @@
         <v>2561</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2640</v>
       </c>
@@ -5929,7 +5927,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2703</v>
       </c>
@@ -5946,7 +5944,7 @@
         <v>2703</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2773</v>
       </c>
@@ -5963,7 +5961,7 @@
         <v>2773</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2832</v>
       </c>
@@ -5980,7 +5978,7 @@
         <v>2832</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2896</v>
       </c>
@@ -5997,7 +5995,7 @@
         <v>2896</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2972</v>
       </c>
@@ -6014,7 +6012,7 @@
         <v>2972</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>3013</v>
       </c>
@@ -6031,7 +6029,7 @@
         <v>3013</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>3135</v>
       </c>
@@ -6048,7 +6046,7 @@
         <v>3135</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>3184</v>
       </c>
@@ -6065,7 +6063,7 @@
         <v>3184</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>3237</v>
       </c>
@@ -6082,7 +6080,7 @@
         <v>3237</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>3286</v>
       </c>
@@ -6099,7 +6097,7 @@
         <v>3286</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>3324</v>
       </c>
@@ -6116,7 +6114,7 @@
         <v>3324</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>3369</v>
       </c>
@@ -6133,7 +6131,7 @@
         <v>3369</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>3416</v>
       </c>
@@ -6150,7 +6148,7 @@
         <v>3416</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>3452</v>
       </c>
@@ -6167,7 +6165,7 @@
         <v>3452</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>3492</v>
       </c>
@@ -6184,7 +6182,7 @@
         <v>3492</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>3530</v>
       </c>
@@ -6201,7 +6199,7 @@
         <v>3530</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>3563</v>
       </c>
@@ -6218,7 +6216,7 @@
         <v>3563</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>3677</v>
       </c>
@@ -6234,7 +6232,7 @@
         <v>3677</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>3876</v>
       </c>
@@ -6250,7 +6248,7 @@
         <v>3876</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>4052</v>
       </c>
@@ -6266,7 +6264,7 @@
         <v>4052</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>4092</v>
       </c>
@@ -6282,12 +6280,12 @@
         <v>4092</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -6301,7 +6299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1197</v>
       </c>
@@ -6317,7 +6315,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1682</v>
       </c>
@@ -6333,7 +6331,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1892</v>
       </c>
@@ -6349,7 +6347,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2164</v>
       </c>
@@ -6365,7 +6363,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2350</v>
       </c>
@@ -6381,7 +6379,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2548</v>
       </c>
@@ -6397,7 +6395,7 @@
         <v>2548</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2740</v>
       </c>
@@ -6413,7 +6411,7 @@
         <v>2740</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2901</v>
       </c>
@@ -6429,7 +6427,7 @@
         <v>2901</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>3096</v>
       </c>
@@ -6445,7 +6443,7 @@
         <v>3096</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>3246</v>
       </c>
@@ -6461,7 +6459,7 @@
         <v>3246</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>3360</v>
       </c>
@@ -6477,7 +6475,7 @@
         <v>3360</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>3503</v>
       </c>
@@ -6493,7 +6491,7 @@
         <v>3503</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>3599</v>
       </c>
@@ -6509,7 +6507,7 @@
         <v>3599</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>3695</v>
       </c>
@@ -6525,7 +6523,7 @@
         <v>3695</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>3880</v>
       </c>
@@ -6541,7 +6539,7 @@
         <v>3880</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>3981</v>
       </c>
@@ -6557,7 +6555,7 @@
         <v>3981</v>
       </c>
     </row>
-    <row r="98" spans="1:12">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>3</v>
       </c>
@@ -6571,7 +6569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:12">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1</v>
       </c>
@@ -6591,7 +6589,7 @@
         <v>1223.1402136155384</v>
       </c>
     </row>
-    <row r="100" spans="1:12">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2</v>
       </c>
@@ -6611,7 +6609,7 @@
         <v>1478.9523243222893</v>
       </c>
     </row>
-    <row r="101" spans="1:12">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>3</v>
       </c>
@@ -6631,7 +6629,7 @@
         <v>1720.8336142805138</v>
       </c>
     </row>
-    <row r="102" spans="1:12">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>4</v>
       </c>
@@ -6653,7 +6651,7 @@
       <c r="H102" s="1"/>
       <c r="L102" s="1"/>
     </row>
-    <row r="103" spans="1:12">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>5</v>
       </c>
@@ -6675,7 +6673,7 @@
       <c r="H103" s="1"/>
       <c r="L103" s="1"/>
     </row>
-    <row r="104" spans="1:12">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>6</v>
       </c>
@@ -6697,7 +6695,7 @@
       <c r="H104" s="1"/>
       <c r="L104" s="1"/>
     </row>
-    <row r="105" spans="1:12">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>7</v>
       </c>
@@ -6719,7 +6717,7 @@
       <c r="H105" s="1"/>
       <c r="L105" s="1"/>
     </row>
-    <row r="106" spans="1:12">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>8</v>
       </c>
@@ -6741,7 +6739,7 @@
       <c r="H106" s="1"/>
       <c r="L106" s="1"/>
     </row>
-    <row r="107" spans="1:12">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>9</v>
       </c>
@@ -6763,7 +6761,7 @@
       <c r="H107" s="1"/>
       <c r="L107" s="1"/>
     </row>
-    <row r="108" spans="1:12">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>10</v>
       </c>
@@ -6785,7 +6783,7 @@
       <c r="H108" s="1"/>
       <c r="L108" s="1"/>
     </row>
-    <row r="109" spans="1:12">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>11</v>
       </c>
@@ -6807,7 +6805,7 @@
       <c r="H109" s="1"/>
       <c r="L109" s="1"/>
     </row>
-    <row r="110" spans="1:12">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>12</v>
       </c>
@@ -6829,7 +6827,7 @@
       <c r="H110" s="1"/>
       <c r="L110" s="1"/>
     </row>
-    <row r="111" spans="1:12">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>13</v>
       </c>
@@ -6851,7 +6849,7 @@
       <c r="H111" s="1"/>
       <c r="L111" s="1"/>
     </row>
-    <row r="112" spans="1:12">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>14</v>
       </c>
@@ -6873,7 +6871,7 @@
       <c r="H112" s="1"/>
       <c r="L112" s="1"/>
     </row>
-    <row r="113" spans="1:12">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>15</v>
       </c>
@@ -6894,7 +6892,7 @@
       <c r="H113" s="1"/>
       <c r="L113" s="1"/>
     </row>
-    <row r="114" spans="1:12">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>16</v>
       </c>
@@ -6915,7 +6913,7 @@
       <c r="H114" s="1"/>
       <c r="L114" s="1"/>
     </row>
-    <row r="115" spans="1:12">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>17</v>
       </c>
@@ -6936,7 +6934,7 @@
       <c r="H115" s="1"/>
       <c r="L115" s="1"/>
     </row>
-    <row r="116" spans="1:12">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>18</v>
       </c>
@@ -6957,7 +6955,7 @@
       <c r="H116" s="1"/>
       <c r="L116" s="1"/>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>19</v>
       </c>
@@ -6978,19 +6976,19 @@
       <c r="H117" s="1"/>
       <c r="L117" s="1"/>
     </row>
-    <row r="118" spans="1:12">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H118" s="1"/>
       <c r="L118" s="1"/>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H119" s="1"/>
       <c r="L119" s="1"/>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H120" s="1"/>
       <c r="L120" s="1"/>
     </row>
-    <row r="123" spans="1:12">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>3</v>
       </c>
@@ -6998,7 +6996,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>1</v>
       </c>
@@ -7026,7 +7024,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:12">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2</v>
       </c>
@@ -7054,7 +7052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:12">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>3</v>
       </c>
@@ -7082,7 +7080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:12">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>4</v>
       </c>
@@ -7110,7 +7108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:12">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>5</v>
       </c>
@@ -7138,7 +7136,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>6</v>
       </c>
@@ -7166,7 +7164,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>7</v>
       </c>
@@ -7194,7 +7192,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>8</v>
       </c>
@@ -7222,7 +7220,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>9</v>
       </c>
@@ -7250,7 +7248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>10</v>
       </c>
@@ -7278,7 +7276,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>11</v>
       </c>
@@ -7306,7 +7304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>12</v>
       </c>
@@ -7334,7 +7332,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>13</v>
       </c>
@@ -7362,7 +7360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>14</v>
       </c>
@@ -7390,7 +7388,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>15</v>
       </c>
@@ -7418,7 +7416,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>16</v>
       </c>
@@ -7446,7 +7444,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>17</v>
       </c>
@@ -7474,7 +7472,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>18</v>
       </c>
@@ -7502,7 +7500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>19</v>
       </c>
@@ -7541,23 +7539,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection activeCell="F79" sqref="F79:J111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -7571,7 +7569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>111</v>
       </c>
@@ -7587,7 +7585,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>132</v>
       </c>
@@ -7603,7 +7601,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>165</v>
       </c>
@@ -7619,7 +7617,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>201</v>
       </c>
@@ -7635,7 +7633,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>248</v>
       </c>
@@ -7651,7 +7649,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>309</v>
       </c>
@@ -7667,7 +7665,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>389</v>
       </c>
@@ -7683,7 +7681,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>485</v>
       </c>
@@ -7699,7 +7697,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>596</v>
       </c>
@@ -7715,7 +7713,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>714</v>
       </c>
@@ -7731,7 +7729,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>894</v>
       </c>
@@ -7747,7 +7745,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1083</v>
       </c>
@@ -7763,7 +7761,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1312</v>
       </c>
@@ -7779,7 +7777,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1539</v>
       </c>
@@ -7795,7 +7793,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1786</v>
       </c>
@@ -7811,7 +7809,7 @@
         <v>1786</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2006</v>
       </c>
@@ -7827,7 +7825,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2208</v>
       </c>
@@ -7843,7 +7841,7 @@
         <v>2208</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2382</v>
       </c>
@@ -7859,7 +7857,7 @@
         <v>2382</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2503</v>
       </c>
@@ -7875,7 +7873,7 @@
         <v>2503</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2602</v>
       </c>
@@ -7891,7 +7889,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2679</v>
       </c>
@@ -7907,7 +7905,7 @@
         <v>2679</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2695</v>
       </c>
@@ -7923,7 +7921,7 @@
         <v>2695</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2728</v>
       </c>
@@ -7939,7 +7937,7 @@
         <v>2728</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2747</v>
       </c>
@@ -7955,7 +7953,7 @@
         <v>2747</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2786</v>
       </c>
@@ -7971,7 +7969,7 @@
         <v>2786</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2824</v>
       </c>
@@ -7987,7 +7985,7 @@
         <v>2824</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2863</v>
       </c>
@@ -8003,7 +8001,7 @@
         <v>2863</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2901</v>
       </c>
@@ -8019,12 +8017,12 @@
         <v>2901</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -8038,7 +8036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>129</v>
       </c>
@@ -8054,7 +8052,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>139</v>
       </c>
@@ -8070,7 +8068,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>149</v>
       </c>
@@ -8086,7 +8084,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>164</v>
       </c>
@@ -8102,7 +8100,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>182</v>
       </c>
@@ -8118,7 +8116,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>191</v>
       </c>
@@ -8134,7 +8132,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>211</v>
       </c>
@@ -8150,7 +8148,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>228</v>
       </c>
@@ -8166,7 +8164,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>251</v>
       </c>
@@ -8182,7 +8180,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>277</v>
       </c>
@@ -8198,7 +8196,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>295</v>
       </c>
@@ -8214,7 +8212,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>326</v>
       </c>
@@ -8230,7 +8228,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>360</v>
       </c>
@@ -8246,7 +8244,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>390</v>
       </c>
@@ -8262,7 +8260,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>430</v>
       </c>
@@ -8278,7 +8276,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>510</v>
       </c>
@@ -8294,7 +8292,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>608</v>
       </c>
@@ -8310,7 +8308,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>706</v>
       </c>
@@ -8326,7 +8324,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>860</v>
       </c>
@@ -8342,7 +8340,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1012</v>
       </c>
@@ -8358,7 +8356,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1171</v>
       </c>
@@ -8374,7 +8372,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1379</v>
       </c>
@@ -8390,7 +8388,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1575</v>
       </c>
@@ -8406,7 +8404,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1737</v>
       </c>
@@ -8422,7 +8420,7 @@
         <v>1737</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1915</v>
       </c>
@@ -8438,7 +8436,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2080</v>
       </c>
@@ -8454,7 +8452,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2197</v>
       </c>
@@ -8470,7 +8468,7 @@
         <v>2197</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2295</v>
       </c>
@@ -8486,7 +8484,7 @@
         <v>2295</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2395</v>
       </c>
@@ -8502,7 +8500,7 @@
         <v>2395</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2450</v>
       </c>
@@ -8518,7 +8516,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2493</v>
       </c>
@@ -8534,7 +8532,7 @@
         <v>2493</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2540</v>
       </c>
@@ -8550,7 +8548,7 @@
         <v>2540</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2579</v>
       </c>
@@ -8566,7 +8564,7 @@
         <v>2579</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2617</v>
       </c>
@@ -8582,7 +8580,7 @@
         <v>2617</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2649</v>
       </c>
@@ -8598,7 +8596,7 @@
         <v>2649</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2699</v>
       </c>
@@ -8614,7 +8612,7 @@
         <v>2699</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2716</v>
       </c>
@@ -8630,7 +8628,7 @@
         <v>2716</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2722</v>
       </c>
@@ -8646,7 +8644,7 @@
         <v>2722</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2734</v>
       </c>
@@ -8662,7 +8660,7 @@
         <v>2734</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2803</v>
       </c>
@@ -8678,7 +8676,7 @@
         <v>2803</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>11</v>
       </c>
@@ -8686,7 +8684,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>1</v>
       </c>
@@ -8714,7 +8712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>2</v>
       </c>
@@ -8742,7 +8740,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="2:10">
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>3</v>
       </c>
@@ -8770,7 +8768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="2:10">
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>4</v>
       </c>
@@ -8798,7 +8796,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="2:10">
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>5</v>
       </c>
@@ -8826,7 +8824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="2:10">
+    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>6</v>
       </c>
@@ -8854,7 +8852,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="2:10">
+    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>7</v>
       </c>
@@ -8882,7 +8880,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="2:10">
+    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>8</v>
       </c>
@@ -8910,7 +8908,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="2:10">
+    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>9</v>
       </c>
@@ -8938,7 +8936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="2:10">
+    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>10</v>
       </c>
@@ -8966,7 +8964,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="2:10">
+    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>11</v>
       </c>
@@ -8994,7 +8992,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="2:10">
+    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>12</v>
       </c>
@@ -9022,7 +9020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="2:10">
+    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>13</v>
       </c>
@@ -9050,7 +9048,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="2:10">
+    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>14</v>
       </c>
@@ -9078,7 +9076,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="2:10">
+    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>15</v>
       </c>
@@ -9106,7 +9104,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="2:10">
+    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>16</v>
       </c>
@@ -9134,7 +9132,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="2:10">
+    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>17</v>
       </c>
@@ -9162,7 +9160,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="2:10">
+    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>18</v>
       </c>
@@ -9190,7 +9188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="2:10">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>19</v>
       </c>
@@ -9218,7 +9216,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="2:10">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>20</v>
       </c>
@@ -9246,7 +9244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="2:10">
+    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>21</v>
       </c>
@@ -9274,7 +9272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="2:10">
+    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>22</v>
       </c>
@@ -9302,7 +9300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="2:10">
+    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>23</v>
       </c>
@@ -9330,7 +9328,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="2:10">
+    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>24</v>
       </c>
@@ -9358,7 +9356,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="2:10">
+    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>25</v>
       </c>
@@ -9386,7 +9384,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="2:10">
+    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>26</v>
       </c>
@@ -9414,7 +9412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="2:10">
+    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B105">
         <v>27</v>
       </c>
@@ -9442,7 +9440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="2:10">
+    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B106">
         <v>28</v>
       </c>
@@ -9470,7 +9468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="2:10">
+    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B107">
         <v>29</v>
       </c>
@@ -9498,7 +9496,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="2:10">
+    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>30</v>
       </c>
@@ -9526,7 +9524,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="2:10">
+    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>31</v>
       </c>
@@ -9554,7 +9552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="2:10">
+    <row r="110" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>32</v>
       </c>
@@ -9582,7 +9580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="2:10">
+    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>33</v>
       </c>
@@ -9610,106 +9608,106 @@
         <v>17</v>
       </c>
     </row>
-    <row r="116" spans="2:7">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" s="3"/>
     </row>
-    <row r="119" spans="2:7">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="2:7">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G120" s="1"/>
     </row>
-    <row r="121" spans="2:7">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G121" s="1"/>
     </row>
-    <row r="122" spans="2:7">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G122" s="1"/>
     </row>
-    <row r="123" spans="2:7">
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G123" s="1"/>
     </row>
-    <row r="124" spans="2:7">
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G124" s="1"/>
     </row>
-    <row r="125" spans="2:7">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G125" s="1"/>
     </row>
-    <row r="126" spans="2:7">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G126" s="1"/>
     </row>
-    <row r="127" spans="2:7">
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G127" s="1"/>
     </row>
-    <row r="128" spans="2:7">
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G128" s="1"/>
     </row>
-    <row r="129" spans="7:7">
+    <row r="129" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G129" s="1"/>
     </row>
-    <row r="130" spans="7:7">
+    <row r="130" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G130" s="1"/>
     </row>
-    <row r="131" spans="7:7">
+    <row r="131" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G131" s="1"/>
     </row>
-    <row r="132" spans="7:7">
+    <row r="132" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G132" s="1"/>
     </row>
-    <row r="133" spans="7:7">
+    <row r="133" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G133" s="1"/>
     </row>
-    <row r="134" spans="7:7">
+    <row r="134" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G134" s="1"/>
     </row>
-    <row r="135" spans="7:7">
+    <row r="135" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G135" s="1"/>
     </row>
-    <row r="136" spans="7:7">
+    <row r="136" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G136" s="1"/>
     </row>
-    <row r="137" spans="7:7">
+    <row r="137" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G137" s="1"/>
     </row>
-    <row r="138" spans="7:7">
+    <row r="138" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G138" s="1"/>
     </row>
-    <row r="139" spans="7:7">
+    <row r="139" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G139" s="1"/>
     </row>
-    <row r="140" spans="7:7">
+    <row r="140" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G140" s="1"/>
     </row>
-    <row r="141" spans="7:7">
+    <row r="141" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G141" s="1"/>
     </row>
-    <row r="142" spans="7:7">
+    <row r="142" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G142" s="1"/>
     </row>
-    <row r="143" spans="7:7">
+    <row r="143" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G143" s="1"/>
     </row>
-    <row r="144" spans="7:7">
+    <row r="144" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G144" s="1"/>
     </row>
-    <row r="145" spans="7:7">
+    <row r="145" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G145" s="1"/>
     </row>
-    <row r="146" spans="7:7">
+    <row r="146" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G146" s="1"/>
     </row>
-    <row r="147" spans="7:7">
+    <row r="147" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G147" s="1"/>
     </row>
-    <row r="148" spans="7:7">
+    <row r="148" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G148" s="1"/>
     </row>
-    <row r="149" spans="7:7">
+    <row r="149" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G149" s="1"/>
     </row>
-    <row r="150" spans="7:7">
+    <row r="150" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G150" s="1"/>
     </row>
-    <row r="151" spans="7:7">
+    <row r="151" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G151" s="1"/>
     </row>
   </sheetData>
@@ -9720,23 +9718,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="5" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -9750,7 +9749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>294</v>
       </c>
@@ -9769,7 +9768,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>375</v>
       </c>
@@ -9780,15 +9779,15 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E29" si="0">B4/8</f>
+        <f t="shared" ref="E4:E30" si="0">B4/8</f>
         <v>300</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F29" si="1">A4</f>
+        <f t="shared" ref="F4:F27" si="1">A4</f>
         <v>375</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>461</v>
       </c>
@@ -9807,7 +9806,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>526</v>
       </c>
@@ -9826,7 +9825,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>601</v>
       </c>
@@ -9845,7 +9844,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>674</v>
       </c>
@@ -9864,7 +9863,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>811</v>
       </c>
@@ -9883,7 +9882,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>925</v>
       </c>
@@ -9902,7 +9901,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1071</v>
       </c>
@@ -9921,7 +9920,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1219</v>
       </c>
@@ -9940,7 +9939,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1445</v>
       </c>
@@ -9959,7 +9958,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1673</v>
       </c>
@@ -9978,7 +9977,7 @@
         <v>1673</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1902</v>
       </c>
@@ -9997,7 +9996,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2187</v>
       </c>
@@ -10016,7 +10015,7 @@
         <v>2187</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2454</v>
       </c>
@@ -10035,7 +10034,7 @@
         <v>2454</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2672</v>
       </c>
@@ -10054,7 +10053,7 @@
         <v>2672</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3000</v>
       </c>
@@ -10073,7 +10072,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3196</v>
       </c>
@@ -10092,7 +10091,7 @@
         <v>3196</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3439</v>
       </c>
@@ -10111,7 +10110,7 @@
         <v>3439</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3583</v>
       </c>
@@ -10130,7 +10129,7 @@
         <v>3583</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3736</v>
       </c>
@@ -10149,7 +10148,7 @@
         <v>3736</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3899</v>
       </c>
@@ -10168,7 +10167,7 @@
         <v>3899</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3960</v>
       </c>
@@ -10187,7 +10186,7 @@
         <v>3960</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4024</v>
       </c>
@@ -10206,7 +10205,7 @@
         <v>4024</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4067</v>
       </c>
@@ -10225,42 +10224,56 @@
         <v>4067</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
+        <f>F28</f>
+        <v>4079</v>
+      </c>
+      <c r="B28">
+        <f>E28*8</f>
+        <v>156</v>
+      </c>
+      <c r="E28">
+        <v>19.5</v>
+      </c>
+      <c r="F28">
+        <v>4079</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>4076</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>0</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>26</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="1"/>
-        <v>4076</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29">
+      <c r="F29">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>4081</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>-160</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>27</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <f t="shared" si="0"/>
         <v>-20</v>
       </c>
-      <c r="F29">
-        <f t="shared" si="1"/>
-        <v>4081</v>
+      <c r="F30">
+        <v>4120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sync with dev branch
change to 1.6.9
</commit_message>
<xml_diff>
--- a/bed-extruder-tables.xlsx
+++ b/bed-extruder-tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bed" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <definedName name="bed1_" localSheetId="0">Bed!$A$80:$B$95</definedName>
     <definedName name="extruder0" localSheetId="1">'Extruder gen 0'!$A$3:$B$30</definedName>
     <definedName name="extruder0_pcb_man" localSheetId="1">'Extruder gen 0'!$A$35:$B$74</definedName>
-    <definedName name="extruder1" localSheetId="2">'Extruder gen 1'!$A$3:$B$29</definedName>
+    <definedName name="extruder1" localSheetId="2">'Extruder gen 1'!$A$3:$B$30</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -144,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -887,11 +887,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91758976"/>
-        <c:axId val="91760512"/>
+        <c:axId val="91271552"/>
+        <c:axId val="91273088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91758976"/>
+        <c:axId val="91271552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -901,12 +901,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91760512"/>
+        <c:crossAx val="91273088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91760512"/>
+        <c:axId val="91273088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -917,7 +917,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91758976"/>
+        <c:crossAx val="91271552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1632,11 +1632,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91792512"/>
-        <c:axId val="91794048"/>
+        <c:axId val="91509888"/>
+        <c:axId val="91511424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91792512"/>
+        <c:axId val="91509888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="160"/>
@@ -1648,12 +1648,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91794048"/>
+        <c:crossAx val="91511424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91794048"/>
+        <c:axId val="91511424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4500"/>
@@ -1666,14 +1666,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91792512"/>
+        <c:crossAx val="91509888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2224,11 +2223,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="93040640"/>
-        <c:axId val="93042560"/>
+        <c:axId val="91631616"/>
+        <c:axId val="91633536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93040640"/>
+        <c:axId val="91631616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="160"/>
@@ -2240,12 +2239,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93042560"/>
+        <c:crossAx val="91633536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93042560"/>
+        <c:axId val="91633536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2256,14 +2255,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93040640"/>
+        <c:crossAx val="91631616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2313,7 +2311,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2742,11 +2739,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="93060096"/>
-        <c:axId val="93065984"/>
+        <c:axId val="91646976"/>
+        <c:axId val="91652864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93060096"/>
+        <c:axId val="91646976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="160"/>
@@ -2758,12 +2755,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93065984"/>
+        <c:crossAx val="91652864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93065984"/>
+        <c:axId val="91652864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2774,14 +2771,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93060096"/>
+        <c:crossAx val="91646976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2826,7 +2822,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3553,11 +3548,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="90898816"/>
-        <c:axId val="90900352"/>
+        <c:axId val="90986368"/>
+        <c:axId val="90987904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90898816"/>
+        <c:axId val="90986368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -3569,12 +3564,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90900352"/>
+        <c:crossAx val="90987904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90900352"/>
+        <c:axId val="90987904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3585,14 +3580,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90898816"/>
+        <c:crossAx val="90986368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3642,7 +3636,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4149,11 +4142,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="90930176"/>
-        <c:axId val="90936064"/>
+        <c:axId val="91026176"/>
+        <c:axId val="91027712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90930176"/>
+        <c:axId val="91026176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4163,12 +4156,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90936064"/>
+        <c:crossAx val="91027712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90936064"/>
+        <c:axId val="91027712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4179,14 +4172,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90930176"/>
+        <c:crossAx val="91026176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4261,10 +4253,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Extruder gen 1'!$E$3:$E$29</c:f>
+              <c:f>'Extruder gen 1'!$E$3:$E$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>320</c:v>
                 </c:pt>
@@ -4341,9 +4333,12 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>-20</c:v>
                 </c:pt>
               </c:numCache>
@@ -4351,10 +4346,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Extruder gen 1'!$F$3:$F$29</c:f>
+              <c:f>'Extruder gen 1'!$F$3:$F$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>294</c:v>
                 </c:pt>
@@ -4431,10 +4426,13 @@
                   <c:v>4067</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4076</c:v>
+                  <c:v>4079</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4081</c:v>
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4449,11 +4447,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="90952832"/>
-        <c:axId val="90954368"/>
+        <c:axId val="91093632"/>
+        <c:axId val="92356992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90952832"/>
+        <c:axId val="91093632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -4465,12 +4463,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90954368"/>
+        <c:crossAx val="92356992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90954368"/>
+        <c:axId val="92356992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4481,7 +4479,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90952832"/>
+        <c:crossAx val="91093632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4702,7 +4700,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4726,15 +4724,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bed0-david" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bed0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bed1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bed0-david" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5042,7 +5040,7 @@
       <selection activeCell="E124" sqref="E124:I142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
@@ -5050,12 +5048,12 @@
     <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5069,7 +5067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2003</v>
       </c>
@@ -5085,7 +5083,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2058</v>
       </c>
@@ -5101,7 +5099,7 @@
         <v>2058</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2161</v>
       </c>
@@ -5117,7 +5115,7 @@
         <v>2161</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2253</v>
       </c>
@@ -5133,7 +5131,7 @@
         <v>2253</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2337</v>
       </c>
@@ -5149,7 +5147,7 @@
         <v>2337</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2450</v>
       </c>
@@ -5165,7 +5163,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2549</v>
       </c>
@@ -5181,7 +5179,7 @@
         <v>2549</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2637</v>
       </c>
@@ -5197,7 +5195,7 @@
         <v>2637</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2715</v>
       </c>
@@ -5213,7 +5211,7 @@
         <v>2715</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2786</v>
       </c>
@@ -5229,7 +5227,7 @@
         <v>2786</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2907</v>
       </c>
@@ -5245,7 +5243,7 @@
         <v>2907</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3008</v>
       </c>
@@ -5261,7 +5259,7 @@
         <v>3008</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3093</v>
       </c>
@@ -5277,7 +5275,7 @@
         <v>3093</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3165</v>
       </c>
@@ -5293,7 +5291,7 @@
         <v>3165</v>
       </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3247</v>
       </c>
@@ -5309,7 +5307,7 @@
         <v>3247</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3316</v>
       </c>
@@ -5331,7 +5329,7 @@
         <v>3708</v>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3374</v>
       </c>
@@ -5353,7 +5351,7 @@
         <v>3816</v>
       </c>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3447</v>
       </c>
@@ -5375,7 +5373,7 @@
         <v>3920</v>
       </c>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3506</v>
       </c>
@@ -5397,7 +5395,7 @@
         <v>4025</v>
       </c>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3548</v>
       </c>
@@ -5419,7 +5417,7 @@
         <v>4129</v>
       </c>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3610</v>
       </c>
@@ -5435,7 +5433,7 @@
         <v>3610</v>
       </c>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3664</v>
       </c>
@@ -5451,7 +5449,7 @@
         <v>3664</v>
       </c>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3708</v>
       </c>
@@ -5467,7 +5465,7 @@
         <v>3708</v>
       </c>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3764</v>
       </c>
@@ -5483,7 +5481,7 @@
         <v>3764</v>
       </c>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3816</v>
       </c>
@@ -5499,7 +5497,7 @@
         <v>3816</v>
       </c>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3868</v>
       </c>
@@ -5515,7 +5513,7 @@
         <v>3868</v>
       </c>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3920</v>
       </c>
@@ -5531,7 +5529,7 @@
         <v>3920</v>
       </c>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4025</v>
       </c>
@@ -5547,7 +5545,7 @@
         <v>4025</v>
       </c>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4129</v>
       </c>
@@ -5563,7 +5561,7 @@
         <v>4129</v>
       </c>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4233</v>
       </c>
@@ -5579,12 +5577,12 @@
         <v>4233</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -5598,7 +5596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -5615,7 +5613,7 @@
       </c>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>180</v>
       </c>
@@ -5631,7 +5629,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>356</v>
       </c>
@@ -5647,7 +5645,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>532</v>
       </c>
@@ -5663,7 +5661,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>708</v>
       </c>
@@ -5679,7 +5677,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>884</v>
       </c>
@@ -5695,7 +5693,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1295</v>
       </c>
@@ -5711,7 +5709,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1306</v>
       </c>
@@ -5727,7 +5725,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1323</v>
       </c>
@@ -5743,7 +5741,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1557</v>
       </c>
@@ -5759,7 +5757,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1755</v>
       </c>
@@ -5776,7 +5774,7 @@
         <v>1755</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2005</v>
       </c>
@@ -5793,7 +5791,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2090</v>
       </c>
@@ -5810,7 +5808,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2151</v>
       </c>
@@ -5827,7 +5825,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2231</v>
       </c>
@@ -5844,7 +5842,7 @@
         <v>2231</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2330</v>
       </c>
@@ -5861,7 +5859,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2398</v>
       </c>
@@ -5878,7 +5876,7 @@
         <v>2398</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2482</v>
       </c>
@@ -5895,7 +5893,7 @@
         <v>2482</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2561</v>
       </c>
@@ -5912,7 +5910,7 @@
         <v>2561</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2640</v>
       </c>
@@ -5929,7 +5927,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2703</v>
       </c>
@@ -5946,7 +5944,7 @@
         <v>2703</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2773</v>
       </c>
@@ -5963,7 +5961,7 @@
         <v>2773</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2832</v>
       </c>
@@ -5980,7 +5978,7 @@
         <v>2832</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2896</v>
       </c>
@@ -5997,7 +5995,7 @@
         <v>2896</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2972</v>
       </c>
@@ -6014,7 +6012,7 @@
         <v>2972</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>3013</v>
       </c>
@@ -6031,7 +6029,7 @@
         <v>3013</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>3135</v>
       </c>
@@ -6048,7 +6046,7 @@
         <v>3135</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>3184</v>
       </c>
@@ -6065,7 +6063,7 @@
         <v>3184</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>3237</v>
       </c>
@@ -6082,7 +6080,7 @@
         <v>3237</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>3286</v>
       </c>
@@ -6099,7 +6097,7 @@
         <v>3286</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>3324</v>
       </c>
@@ -6116,7 +6114,7 @@
         <v>3324</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>3369</v>
       </c>
@@ -6133,7 +6131,7 @@
         <v>3369</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>3416</v>
       </c>
@@ -6150,7 +6148,7 @@
         <v>3416</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>3452</v>
       </c>
@@ -6167,7 +6165,7 @@
         <v>3452</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>3492</v>
       </c>
@@ -6184,7 +6182,7 @@
         <v>3492</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>3530</v>
       </c>
@@ -6201,7 +6199,7 @@
         <v>3530</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>3563</v>
       </c>
@@ -6218,7 +6216,7 @@
         <v>3563</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>3677</v>
       </c>
@@ -6234,7 +6232,7 @@
         <v>3677</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>3876</v>
       </c>
@@ -6250,7 +6248,7 @@
         <v>3876</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>4052</v>
       </c>
@@ -6266,7 +6264,7 @@
         <v>4052</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>4092</v>
       </c>
@@ -6282,12 +6280,12 @@
         <v>4092</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -6301,7 +6299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1197</v>
       </c>
@@ -6317,7 +6315,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1682</v>
       </c>
@@ -6333,7 +6331,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1892</v>
       </c>
@@ -6349,7 +6347,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2164</v>
       </c>
@@ -6365,7 +6363,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2350</v>
       </c>
@@ -6381,7 +6379,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2548</v>
       </c>
@@ -6397,7 +6395,7 @@
         <v>2548</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2740</v>
       </c>
@@ -6413,7 +6411,7 @@
         <v>2740</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2901</v>
       </c>
@@ -6429,7 +6427,7 @@
         <v>2901</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>3096</v>
       </c>
@@ -6445,7 +6443,7 @@
         <v>3096</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>3246</v>
       </c>
@@ -6461,7 +6459,7 @@
         <v>3246</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>3360</v>
       </c>
@@ -6477,7 +6475,7 @@
         <v>3360</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>3503</v>
       </c>
@@ -6493,7 +6491,7 @@
         <v>3503</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>3599</v>
       </c>
@@ -6509,7 +6507,7 @@
         <v>3599</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>3695</v>
       </c>
@@ -6525,7 +6523,7 @@
         <v>3695</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>3880</v>
       </c>
@@ -6541,7 +6539,7 @@
         <v>3880</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>3981</v>
       </c>
@@ -6557,7 +6555,7 @@
         <v>3981</v>
       </c>
     </row>
-    <row r="98" spans="1:12">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>3</v>
       </c>
@@ -6571,7 +6569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:12">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1</v>
       </c>
@@ -6591,7 +6589,7 @@
         <v>1223.1402136155384</v>
       </c>
     </row>
-    <row r="100" spans="1:12">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2</v>
       </c>
@@ -6611,7 +6609,7 @@
         <v>1478.9523243222893</v>
       </c>
     </row>
-    <row r="101" spans="1:12">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>3</v>
       </c>
@@ -6631,7 +6629,7 @@
         <v>1720.8336142805138</v>
       </c>
     </row>
-    <row r="102" spans="1:12">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>4</v>
       </c>
@@ -6653,7 +6651,7 @@
       <c r="H102" s="1"/>
       <c r="L102" s="1"/>
     </row>
-    <row r="103" spans="1:12">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>5</v>
       </c>
@@ -6675,7 +6673,7 @@
       <c r="H103" s="1"/>
       <c r="L103" s="1"/>
     </row>
-    <row r="104" spans="1:12">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>6</v>
       </c>
@@ -6697,7 +6695,7 @@
       <c r="H104" s="1"/>
       <c r="L104" s="1"/>
     </row>
-    <row r="105" spans="1:12">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>7</v>
       </c>
@@ -6719,7 +6717,7 @@
       <c r="H105" s="1"/>
       <c r="L105" s="1"/>
     </row>
-    <row r="106" spans="1:12">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>8</v>
       </c>
@@ -6741,7 +6739,7 @@
       <c r="H106" s="1"/>
       <c r="L106" s="1"/>
     </row>
-    <row r="107" spans="1:12">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>9</v>
       </c>
@@ -6763,7 +6761,7 @@
       <c r="H107" s="1"/>
       <c r="L107" s="1"/>
     </row>
-    <row r="108" spans="1:12">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>10</v>
       </c>
@@ -6785,7 +6783,7 @@
       <c r="H108" s="1"/>
       <c r="L108" s="1"/>
     </row>
-    <row r="109" spans="1:12">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>11</v>
       </c>
@@ -6807,7 +6805,7 @@
       <c r="H109" s="1"/>
       <c r="L109" s="1"/>
     </row>
-    <row r="110" spans="1:12">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>12</v>
       </c>
@@ -6829,7 +6827,7 @@
       <c r="H110" s="1"/>
       <c r="L110" s="1"/>
     </row>
-    <row r="111" spans="1:12">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>13</v>
       </c>
@@ -6851,7 +6849,7 @@
       <c r="H111" s="1"/>
       <c r="L111" s="1"/>
     </row>
-    <row r="112" spans="1:12">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>14</v>
       </c>
@@ -6873,7 +6871,7 @@
       <c r="H112" s="1"/>
       <c r="L112" s="1"/>
     </row>
-    <row r="113" spans="1:12">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>15</v>
       </c>
@@ -6894,7 +6892,7 @@
       <c r="H113" s="1"/>
       <c r="L113" s="1"/>
     </row>
-    <row r="114" spans="1:12">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>16</v>
       </c>
@@ -6915,7 +6913,7 @@
       <c r="H114" s="1"/>
       <c r="L114" s="1"/>
     </row>
-    <row r="115" spans="1:12">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>17</v>
       </c>
@@ -6936,7 +6934,7 @@
       <c r="H115" s="1"/>
       <c r="L115" s="1"/>
     </row>
-    <row r="116" spans="1:12">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>18</v>
       </c>
@@ -6957,7 +6955,7 @@
       <c r="H116" s="1"/>
       <c r="L116" s="1"/>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>19</v>
       </c>
@@ -6978,19 +6976,19 @@
       <c r="H117" s="1"/>
       <c r="L117" s="1"/>
     </row>
-    <row r="118" spans="1:12">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H118" s="1"/>
       <c r="L118" s="1"/>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H119" s="1"/>
       <c r="L119" s="1"/>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H120" s="1"/>
       <c r="L120" s="1"/>
     </row>
-    <row r="123" spans="1:12">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>3</v>
       </c>
@@ -6998,7 +6996,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>1</v>
       </c>
@@ -7026,7 +7024,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:12">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2</v>
       </c>
@@ -7054,7 +7052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:12">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>3</v>
       </c>
@@ -7082,7 +7080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:12">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>4</v>
       </c>
@@ -7110,7 +7108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:12">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>5</v>
       </c>
@@ -7138,7 +7136,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>6</v>
       </c>
@@ -7166,7 +7164,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>7</v>
       </c>
@@ -7194,7 +7192,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>8</v>
       </c>
@@ -7222,7 +7220,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>9</v>
       </c>
@@ -7250,7 +7248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>10</v>
       </c>
@@ -7278,7 +7276,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>11</v>
       </c>
@@ -7306,7 +7304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>12</v>
       </c>
@@ -7334,7 +7332,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>13</v>
       </c>
@@ -7362,7 +7360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>14</v>
       </c>
@@ -7390,7 +7388,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>15</v>
       </c>
@@ -7418,7 +7416,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>16</v>
       </c>
@@ -7446,7 +7444,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>17</v>
       </c>
@@ -7474,7 +7472,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>18</v>
       </c>
@@ -7502,7 +7500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>19</v>
       </c>
@@ -7541,23 +7539,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection activeCell="F79" sqref="F79:J111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -7571,7 +7569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>111</v>
       </c>
@@ -7587,7 +7585,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>132</v>
       </c>
@@ -7603,7 +7601,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>165</v>
       </c>
@@ -7619,7 +7617,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>201</v>
       </c>
@@ -7635,7 +7633,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>248</v>
       </c>
@@ -7651,7 +7649,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>309</v>
       </c>
@@ -7667,7 +7665,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>389</v>
       </c>
@@ -7683,7 +7681,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>485</v>
       </c>
@@ -7699,7 +7697,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>596</v>
       </c>
@@ -7715,7 +7713,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>714</v>
       </c>
@@ -7731,7 +7729,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>894</v>
       </c>
@@ -7747,7 +7745,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1083</v>
       </c>
@@ -7763,7 +7761,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1312</v>
       </c>
@@ -7779,7 +7777,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1539</v>
       </c>
@@ -7795,7 +7793,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1786</v>
       </c>
@@ -7811,7 +7809,7 @@
         <v>1786</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2006</v>
       </c>
@@ -7827,7 +7825,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2208</v>
       </c>
@@ -7843,7 +7841,7 @@
         <v>2208</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2382</v>
       </c>
@@ -7859,7 +7857,7 @@
         <v>2382</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2503</v>
       </c>
@@ -7875,7 +7873,7 @@
         <v>2503</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2602</v>
       </c>
@@ -7891,7 +7889,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2679</v>
       </c>
@@ -7907,7 +7905,7 @@
         <v>2679</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2695</v>
       </c>
@@ -7923,7 +7921,7 @@
         <v>2695</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2728</v>
       </c>
@@ -7939,7 +7937,7 @@
         <v>2728</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2747</v>
       </c>
@@ -7955,7 +7953,7 @@
         <v>2747</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2786</v>
       </c>
@@ -7971,7 +7969,7 @@
         <v>2786</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2824</v>
       </c>
@@ -7987,7 +7985,7 @@
         <v>2824</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2863</v>
       </c>
@@ -8003,7 +8001,7 @@
         <v>2863</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2901</v>
       </c>
@@ -8019,12 +8017,12 @@
         <v>2901</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -8038,7 +8036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>129</v>
       </c>
@@ -8054,7 +8052,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>139</v>
       </c>
@@ -8070,7 +8068,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>149</v>
       </c>
@@ -8086,7 +8084,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>164</v>
       </c>
@@ -8102,7 +8100,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>182</v>
       </c>
@@ -8118,7 +8116,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>191</v>
       </c>
@@ -8134,7 +8132,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>211</v>
       </c>
@@ -8150,7 +8148,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>228</v>
       </c>
@@ -8166,7 +8164,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>251</v>
       </c>
@@ -8182,7 +8180,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>277</v>
       </c>
@@ -8198,7 +8196,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>295</v>
       </c>
@@ -8214,7 +8212,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>326</v>
       </c>
@@ -8230,7 +8228,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>360</v>
       </c>
@@ -8246,7 +8244,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>390</v>
       </c>
@@ -8262,7 +8260,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>430</v>
       </c>
@@ -8278,7 +8276,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>510</v>
       </c>
@@ -8294,7 +8292,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>608</v>
       </c>
@@ -8310,7 +8308,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>706</v>
       </c>
@@ -8326,7 +8324,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>860</v>
       </c>
@@ -8342,7 +8340,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1012</v>
       </c>
@@ -8358,7 +8356,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1171</v>
       </c>
@@ -8374,7 +8372,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1379</v>
       </c>
@@ -8390,7 +8388,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1575</v>
       </c>
@@ -8406,7 +8404,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1737</v>
       </c>
@@ -8422,7 +8420,7 @@
         <v>1737</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1915</v>
       </c>
@@ -8438,7 +8436,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2080</v>
       </c>
@@ -8454,7 +8452,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2197</v>
       </c>
@@ -8470,7 +8468,7 @@
         <v>2197</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2295</v>
       </c>
@@ -8486,7 +8484,7 @@
         <v>2295</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2395</v>
       </c>
@@ -8502,7 +8500,7 @@
         <v>2395</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2450</v>
       </c>
@@ -8518,7 +8516,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2493</v>
       </c>
@@ -8534,7 +8532,7 @@
         <v>2493</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2540</v>
       </c>
@@ -8550,7 +8548,7 @@
         <v>2540</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2579</v>
       </c>
@@ -8566,7 +8564,7 @@
         <v>2579</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2617</v>
       </c>
@@ -8582,7 +8580,7 @@
         <v>2617</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2649</v>
       </c>
@@ -8598,7 +8596,7 @@
         <v>2649</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2699</v>
       </c>
@@ -8614,7 +8612,7 @@
         <v>2699</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2716</v>
       </c>
@@ -8630,7 +8628,7 @@
         <v>2716</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2722</v>
       </c>
@@ -8646,7 +8644,7 @@
         <v>2722</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2734</v>
       </c>
@@ -8662,7 +8660,7 @@
         <v>2734</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2803</v>
       </c>
@@ -8678,7 +8676,7 @@
         <v>2803</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>11</v>
       </c>
@@ -8686,7 +8684,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>1</v>
       </c>
@@ -8714,7 +8712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>2</v>
       </c>
@@ -8742,7 +8740,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="2:10">
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>3</v>
       </c>
@@ -8770,7 +8768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="2:10">
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>4</v>
       </c>
@@ -8798,7 +8796,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="2:10">
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>5</v>
       </c>
@@ -8826,7 +8824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="2:10">
+    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>6</v>
       </c>
@@ -8854,7 +8852,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="2:10">
+    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>7</v>
       </c>
@@ -8882,7 +8880,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="2:10">
+    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>8</v>
       </c>
@@ -8910,7 +8908,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="2:10">
+    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>9</v>
       </c>
@@ -8938,7 +8936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="2:10">
+    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>10</v>
       </c>
@@ -8966,7 +8964,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="2:10">
+    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>11</v>
       </c>
@@ -8994,7 +8992,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="2:10">
+    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>12</v>
       </c>
@@ -9022,7 +9020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="2:10">
+    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>13</v>
       </c>
@@ -9050,7 +9048,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="2:10">
+    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>14</v>
       </c>
@@ -9078,7 +9076,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="2:10">
+    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>15</v>
       </c>
@@ -9106,7 +9104,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="2:10">
+    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>16</v>
       </c>
@@ -9134,7 +9132,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="2:10">
+    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>17</v>
       </c>
@@ -9162,7 +9160,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="2:10">
+    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>18</v>
       </c>
@@ -9190,7 +9188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="2:10">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>19</v>
       </c>
@@ -9218,7 +9216,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="2:10">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>20</v>
       </c>
@@ -9246,7 +9244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="2:10">
+    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>21</v>
       </c>
@@ -9274,7 +9272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="2:10">
+    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>22</v>
       </c>
@@ -9302,7 +9300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="2:10">
+    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>23</v>
       </c>
@@ -9330,7 +9328,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="2:10">
+    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>24</v>
       </c>
@@ -9358,7 +9356,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="2:10">
+    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>25</v>
       </c>
@@ -9386,7 +9384,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="2:10">
+    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>26</v>
       </c>
@@ -9414,7 +9412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="2:10">
+    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B105">
         <v>27</v>
       </c>
@@ -9442,7 +9440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="2:10">
+    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B106">
         <v>28</v>
       </c>
@@ -9470,7 +9468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="2:10">
+    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B107">
         <v>29</v>
       </c>
@@ -9498,7 +9496,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="2:10">
+    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>30</v>
       </c>
@@ -9526,7 +9524,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="2:10">
+    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>31</v>
       </c>
@@ -9554,7 +9552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="2:10">
+    <row r="110" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>32</v>
       </c>
@@ -9582,7 +9580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="2:10">
+    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>33</v>
       </c>
@@ -9610,106 +9608,106 @@
         <v>17</v>
       </c>
     </row>
-    <row r="116" spans="2:7">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" s="3"/>
     </row>
-    <row r="119" spans="2:7">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="2:7">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G120" s="1"/>
     </row>
-    <row r="121" spans="2:7">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G121" s="1"/>
     </row>
-    <row r="122" spans="2:7">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G122" s="1"/>
     </row>
-    <row r="123" spans="2:7">
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G123" s="1"/>
     </row>
-    <row r="124" spans="2:7">
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G124" s="1"/>
     </row>
-    <row r="125" spans="2:7">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G125" s="1"/>
     </row>
-    <row r="126" spans="2:7">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G126" s="1"/>
     </row>
-    <row r="127" spans="2:7">
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G127" s="1"/>
     </row>
-    <row r="128" spans="2:7">
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G128" s="1"/>
     </row>
-    <row r="129" spans="7:7">
+    <row r="129" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G129" s="1"/>
     </row>
-    <row r="130" spans="7:7">
+    <row r="130" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G130" s="1"/>
     </row>
-    <row r="131" spans="7:7">
+    <row r="131" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G131" s="1"/>
     </row>
-    <row r="132" spans="7:7">
+    <row r="132" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G132" s="1"/>
     </row>
-    <row r="133" spans="7:7">
+    <row r="133" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G133" s="1"/>
     </row>
-    <row r="134" spans="7:7">
+    <row r="134" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G134" s="1"/>
     </row>
-    <row r="135" spans="7:7">
+    <row r="135" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G135" s="1"/>
     </row>
-    <row r="136" spans="7:7">
+    <row r="136" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G136" s="1"/>
     </row>
-    <row r="137" spans="7:7">
+    <row r="137" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G137" s="1"/>
     </row>
-    <row r="138" spans="7:7">
+    <row r="138" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G138" s="1"/>
     </row>
-    <row r="139" spans="7:7">
+    <row r="139" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G139" s="1"/>
     </row>
-    <row r="140" spans="7:7">
+    <row r="140" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G140" s="1"/>
     </row>
-    <row r="141" spans="7:7">
+    <row r="141" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G141" s="1"/>
     </row>
-    <row r="142" spans="7:7">
+    <row r="142" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G142" s="1"/>
     </row>
-    <row r="143" spans="7:7">
+    <row r="143" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G143" s="1"/>
     </row>
-    <row r="144" spans="7:7">
+    <row r="144" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G144" s="1"/>
     </row>
-    <row r="145" spans="7:7">
+    <row r="145" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G145" s="1"/>
     </row>
-    <row r="146" spans="7:7">
+    <row r="146" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G146" s="1"/>
     </row>
-    <row r="147" spans="7:7">
+    <row r="147" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G147" s="1"/>
     </row>
-    <row r="148" spans="7:7">
+    <row r="148" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G148" s="1"/>
     </row>
-    <row r="149" spans="7:7">
+    <row r="149" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G149" s="1"/>
     </row>
-    <row r="150" spans="7:7">
+    <row r="150" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G150" s="1"/>
     </row>
-    <row r="151" spans="7:7">
+    <row r="151" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G151" s="1"/>
     </row>
   </sheetData>
@@ -9720,23 +9718,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="5" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -9750,7 +9749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>294</v>
       </c>
@@ -9769,7 +9768,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>375</v>
       </c>
@@ -9780,15 +9779,15 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E29" si="0">B4/8</f>
+        <f t="shared" ref="E4:E30" si="0">B4/8</f>
         <v>300</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F29" si="1">A4</f>
+        <f t="shared" ref="F4:F27" si="1">A4</f>
         <v>375</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>461</v>
       </c>
@@ -9807,7 +9806,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>526</v>
       </c>
@@ -9826,7 +9825,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>601</v>
       </c>
@@ -9845,7 +9844,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>674</v>
       </c>
@@ -9864,7 +9863,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>811</v>
       </c>
@@ -9883,7 +9882,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>925</v>
       </c>
@@ -9902,7 +9901,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1071</v>
       </c>
@@ -9921,7 +9920,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1219</v>
       </c>
@@ -9940,7 +9939,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1445</v>
       </c>
@@ -9959,7 +9958,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1673</v>
       </c>
@@ -9978,7 +9977,7 @@
         <v>1673</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1902</v>
       </c>
@@ -9997,7 +9996,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2187</v>
       </c>
@@ -10016,7 +10015,7 @@
         <v>2187</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2454</v>
       </c>
@@ -10035,7 +10034,7 @@
         <v>2454</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2672</v>
       </c>
@@ -10054,7 +10053,7 @@
         <v>2672</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3000</v>
       </c>
@@ -10073,7 +10072,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3196</v>
       </c>
@@ -10092,7 +10091,7 @@
         <v>3196</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3439</v>
       </c>
@@ -10111,7 +10110,7 @@
         <v>3439</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3583</v>
       </c>
@@ -10130,7 +10129,7 @@
         <v>3583</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3736</v>
       </c>
@@ -10149,7 +10148,7 @@
         <v>3736</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3899</v>
       </c>
@@ -10168,7 +10167,7 @@
         <v>3899</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3960</v>
       </c>
@@ -10187,7 +10186,7 @@
         <v>3960</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4024</v>
       </c>
@@ -10206,7 +10205,7 @@
         <v>4024</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4067</v>
       </c>
@@ -10225,42 +10224,56 @@
         <v>4067</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
+        <f>F28</f>
+        <v>4079</v>
+      </c>
+      <c r="B28">
+        <f>E28*8</f>
+        <v>156</v>
+      </c>
+      <c r="E28">
+        <v>19.5</v>
+      </c>
+      <c r="F28">
+        <v>4079</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>4076</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>0</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>26</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="1"/>
-        <v>4076</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29">
+      <c r="F29">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>4081</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>-160</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>27</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <f t="shared" si="0"/>
         <v>-20</v>
       </c>
-      <c r="F29">
-        <f t="shared" si="1"/>
-        <v>4081</v>
+      <c r="F30">
+        <v>4120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>